<commit_message>
Adicionando a melhor documentação que já existiu pra um sistema
</commit_message>
<xml_diff>
--- a/funcionalidades.xlsx
+++ b/funcionalidades.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="323">
   <si>
     <t>Profissionais</t>
   </si>
@@ -982,6 +982,9 @@
   </si>
   <si>
     <t>Link para gráficos (Invisível)</t>
+  </si>
+  <si>
+    <t>Filter de verificação de pagamento (402)</t>
   </si>
 </sst>
 </file>
@@ -1330,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E263"/>
+  <dimension ref="A1:E264"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3396,7 +3399,7 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" t="s">
-        <v>143</v>
+        <v>322</v>
       </c>
       <c r="B122" t="s">
         <v>2</v>
@@ -3413,7 +3416,7 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="B123" t="s">
         <v>2</v>
@@ -3430,7 +3433,7 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B124" t="s">
         <v>2</v>
@@ -3447,7 +3450,7 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B125" t="s">
         <v>2</v>
@@ -3464,7 +3467,7 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="B126" t="s">
         <v>2</v>
@@ -3481,7 +3484,7 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B127" t="s">
         <v>2</v>
@@ -3498,7 +3501,7 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B128" t="s">
         <v>2</v>
@@ -3515,7 +3518,7 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B129" t="s">
         <v>2</v>
@@ -3532,7 +3535,7 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B130" t="s">
         <v>2</v>
@@ -3549,7 +3552,7 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B131" t="s">
         <v>2</v>
@@ -3566,7 +3569,7 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B132" t="s">
         <v>2</v>
@@ -3583,7 +3586,7 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B133" t="s">
         <v>2</v>
@@ -3600,7 +3603,7 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B134" t="s">
         <v>2</v>
@@ -3617,7 +3620,7 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>220</v>
+        <v>158</v>
       </c>
       <c r="B135" t="s">
         <v>2</v>
@@ -3634,7 +3637,7 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B136" t="s">
         <v>2</v>
@@ -3651,7 +3654,7 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B137" t="s">
         <v>2</v>
@@ -3668,13 +3671,13 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>116</v>
+        <v>222</v>
       </c>
       <c r="B138" t="s">
-        <v>188</v>
+        <v>2</v>
       </c>
       <c r="C138" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="D138">
         <v>1</v>
@@ -3685,7 +3688,7 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B139" t="s">
         <v>188</v>
@@ -3702,7 +3705,7 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="B140" t="s">
         <v>188</v>
@@ -3719,7 +3722,7 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B141" t="s">
         <v>188</v>
@@ -3736,16 +3739,16 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="B142" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C142" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D142">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E142" t="s">
         <v>185</v>
@@ -3753,7 +3756,7 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B143" t="s">
         <v>189</v>
@@ -3770,16 +3773,16 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="B144" t="s">
-        <v>1</v>
+        <v>189</v>
       </c>
       <c r="C144" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="D144">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E144" t="s">
         <v>185</v>
@@ -3787,7 +3790,7 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" t="s">
-        <v>162</v>
+        <v>33</v>
       </c>
       <c r="B145" t="s">
         <v>1</v>
@@ -3804,7 +3807,7 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B146" t="s">
         <v>1</v>
@@ -3821,7 +3824,7 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" t="s">
-        <v>70</v>
+        <v>167</v>
       </c>
       <c r="B147" t="s">
         <v>1</v>
@@ -3838,7 +3841,7 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="B148" t="s">
         <v>1</v>
@@ -3855,7 +3858,7 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="B149" t="s">
         <v>1</v>
@@ -3872,7 +3875,7 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B150" t="s">
         <v>1</v>
@@ -3889,7 +3892,7 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B151" t="s">
         <v>1</v>
@@ -3906,7 +3909,7 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B152" t="s">
         <v>1</v>
@@ -3923,7 +3926,7 @@
     </row>
     <row r="153" spans="1:5">
       <c r="A153" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B153" t="s">
         <v>1</v>
@@ -3940,7 +3943,7 @@
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B154" t="s">
         <v>1</v>
@@ -3957,7 +3960,7 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B155" t="s">
         <v>1</v>
@@ -3974,7 +3977,7 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B156" t="s">
         <v>1</v>
@@ -3991,7 +3994,7 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B157" t="s">
         <v>1</v>
@@ -4008,7 +4011,7 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B158" t="s">
         <v>1</v>
@@ -4025,7 +4028,7 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B159" t="s">
         <v>1</v>
@@ -4042,7 +4045,7 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B160" t="s">
         <v>1</v>
@@ -4059,7 +4062,7 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B161" t="s">
         <v>1</v>
@@ -4076,7 +4079,7 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" t="s">
-        <v>227</v>
+        <v>66</v>
       </c>
       <c r="B162" t="s">
         <v>1</v>
@@ -4093,7 +4096,7 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B163" t="s">
         <v>1</v>
@@ -4110,7 +4113,7 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="B164" t="s">
         <v>1</v>
@@ -4127,7 +4130,7 @@
     </row>
     <row r="165" spans="1:5">
       <c r="A165" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B165" t="s">
         <v>1</v>
@@ -4144,7 +4147,7 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B166" t="s">
         <v>1</v>
@@ -4161,30 +4164,30 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="B167" t="s">
-        <v>188</v>
+        <v>1</v>
       </c>
       <c r="C167" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="D167">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E167" t="s">
-        <v>115</v>
+        <v>185</v>
       </c>
     </row>
     <row r="168" spans="1:5">
       <c r="A168" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B168" t="s">
         <v>188</v>
       </c>
       <c r="C168" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D168">
         <v>1</v>
@@ -4195,16 +4198,16 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="B169" t="s">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="C169" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D169">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E169" t="s">
         <v>115</v>
@@ -4212,7 +4215,7 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B170" t="s">
         <v>1</v>
@@ -4229,7 +4232,7 @@
     </row>
     <row r="171" spans="1:5">
       <c r="A171" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B171" t="s">
         <v>1</v>
@@ -4246,7 +4249,7 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B172" t="s">
         <v>1</v>
@@ -4263,7 +4266,7 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B173" t="s">
         <v>1</v>
@@ -4280,7 +4283,7 @@
     </row>
     <row r="174" spans="1:5">
       <c r="A174" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B174" t="s">
         <v>1</v>
@@ -4297,16 +4300,16 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="B175" t="s">
         <v>1</v>
       </c>
       <c r="C175" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D175">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E175" t="s">
         <v>115</v>
@@ -4314,7 +4317,7 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B176" t="s">
         <v>1</v>
@@ -4331,7 +4334,7 @@
     </row>
     <row r="177" spans="1:5">
       <c r="A177" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B177" t="s">
         <v>1</v>
@@ -4348,7 +4351,7 @@
     </row>
     <row r="178" spans="1:5">
       <c r="A178" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B178" t="s">
         <v>1</v>
@@ -4365,7 +4368,7 @@
     </row>
     <row r="179" spans="1:5">
       <c r="A179" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B179" t="s">
         <v>1</v>
@@ -4382,7 +4385,7 @@
     </row>
     <row r="180" spans="1:5">
       <c r="A180" t="s">
-        <v>169</v>
+        <v>72</v>
       </c>
       <c r="B180" t="s">
         <v>1</v>
@@ -4399,7 +4402,7 @@
     </row>
     <row r="181" spans="1:5">
       <c r="A181" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="B181" t="s">
         <v>1</v>
@@ -4416,7 +4419,7 @@
     </row>
     <row r="182" spans="1:5">
       <c r="A182" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B182" t="s">
         <v>1</v>
@@ -4433,7 +4436,7 @@
     </row>
     <row r="183" spans="1:5">
       <c r="A183" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B183" t="s">
         <v>1</v>
@@ -4450,7 +4453,7 @@
     </row>
     <row r="184" spans="1:5">
       <c r="A184" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B184" t="s">
         <v>1</v>
@@ -4467,7 +4470,7 @@
     </row>
     <row r="185" spans="1:5">
       <c r="A185" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B185" t="s">
         <v>1</v>
@@ -4484,24 +4487,24 @@
     </row>
     <row r="186" spans="1:5">
       <c r="A186" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B186" t="s">
         <v>1</v>
       </c>
       <c r="C186" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="D186">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E186" t="s">
-        <v>205</v>
+        <v>115</v>
       </c>
     </row>
     <row r="187" spans="1:5">
       <c r="A187" t="s">
-        <v>242</v>
+        <v>134</v>
       </c>
       <c r="B187" t="s">
         <v>1</v>
@@ -4518,7 +4521,7 @@
     </row>
     <row r="188" spans="1:5">
       <c r="A188" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B188" t="s">
         <v>1</v>
@@ -4535,7 +4538,7 @@
     </row>
     <row r="189" spans="1:5">
       <c r="A189" t="s">
-        <v>199</v>
+        <v>236</v>
       </c>
       <c r="B189" t="s">
         <v>1</v>
@@ -4552,13 +4555,13 @@
     </row>
     <row r="190" spans="1:5">
       <c r="A190" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="B190" t="s">
         <v>1</v>
       </c>
       <c r="C190" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="D190">
         <v>1</v>
@@ -4569,16 +4572,16 @@
     </row>
     <row r="191" spans="1:5">
       <c r="A191" t="s">
-        <v>8</v>
+        <v>159</v>
       </c>
       <c r="B191" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C191" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="D191">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E191" t="s">
         <v>205</v>
@@ -4586,7 +4589,7 @@
     </row>
     <row r="192" spans="1:5">
       <c r="A192" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B192" t="s">
         <v>0</v>
@@ -4603,7 +4606,7 @@
     </row>
     <row r="193" spans="1:5">
       <c r="A193" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="B193" t="s">
         <v>0</v>
@@ -4620,7 +4623,7 @@
     </row>
     <row r="194" spans="1:5">
       <c r="A194" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B194" t="s">
         <v>0</v>
@@ -4637,7 +4640,7 @@
     </row>
     <row r="195" spans="1:5">
       <c r="A195" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B195" t="s">
         <v>0</v>
@@ -4654,16 +4657,16 @@
     </row>
     <row r="196" spans="1:5">
       <c r="A196" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B196" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C196" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="D196">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E196" t="s">
         <v>205</v>
@@ -4671,7 +4674,7 @@
     </row>
     <row r="197" spans="1:5">
       <c r="A197" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B197" t="s">
         <v>1</v>
@@ -4688,7 +4691,7 @@
     </row>
     <row r="198" spans="1:5">
       <c r="A198" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B198" t="s">
         <v>1</v>
@@ -4705,7 +4708,7 @@
     </row>
     <row r="199" spans="1:5">
       <c r="A199" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B199" t="s">
         <v>1</v>
@@ -4722,7 +4725,7 @@
     </row>
     <row r="200" spans="1:5">
       <c r="A200" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B200" t="s">
         <v>1</v>
@@ -4739,7 +4742,7 @@
     </row>
     <row r="201" spans="1:5">
       <c r="A201" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B201" t="s">
         <v>1</v>
@@ -4756,7 +4759,7 @@
     </row>
     <row r="202" spans="1:5">
       <c r="A202" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B202" t="s">
         <v>1</v>
@@ -4773,16 +4776,16 @@
     </row>
     <row r="203" spans="1:5">
       <c r="A203" t="s">
-        <v>237</v>
+        <v>50</v>
       </c>
       <c r="B203" t="s">
-        <v>188</v>
+        <v>1</v>
       </c>
       <c r="C203" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D203">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E203" t="s">
         <v>205</v>
@@ -4790,7 +4793,7 @@
     </row>
     <row r="204" spans="1:5">
       <c r="A204" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B204" t="s">
         <v>188</v>
@@ -4807,7 +4810,7 @@
     </row>
     <row r="205" spans="1:5">
       <c r="A205" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B205" t="s">
         <v>188</v>
@@ -4824,7 +4827,7 @@
     </row>
     <row r="206" spans="1:5">
       <c r="A206" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B206" t="s">
         <v>188</v>
@@ -4841,24 +4844,24 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207" t="s">
-        <v>130</v>
+        <v>240</v>
       </c>
       <c r="B207" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C207" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D207">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E207" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
     </row>
     <row r="208" spans="1:5">
       <c r="A208" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B208" t="s">
         <v>189</v>
@@ -4875,7 +4878,7 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="B209" t="s">
         <v>189</v>
@@ -4892,7 +4895,7 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B210" t="s">
         <v>189</v>
@@ -4909,7 +4912,7 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B211" t="s">
         <v>189</v>
@@ -4926,7 +4929,7 @@
     </row>
     <row r="212" spans="1:5">
       <c r="A212" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B212" t="s">
         <v>189</v>
@@ -4943,7 +4946,7 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B213" t="s">
         <v>189</v>
@@ -4960,7 +4963,7 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B214" t="s">
         <v>189</v>
@@ -4977,7 +4980,7 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B215" t="s">
         <v>189</v>
@@ -4994,7 +4997,7 @@
     </row>
     <row r="216" spans="1:5">
       <c r="A216" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B216" t="s">
         <v>189</v>
@@ -5011,7 +5014,7 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B217" t="s">
         <v>189</v>
@@ -5028,7 +5031,7 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="B218" t="s">
         <v>189</v>
@@ -5045,7 +5048,7 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="B219" t="s">
         <v>189</v>
@@ -5062,7 +5065,7 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B220" t="s">
         <v>189</v>
@@ -5079,7 +5082,7 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="B221" t="s">
         <v>189</v>
@@ -5096,16 +5099,16 @@
     </row>
     <row r="222" spans="1:5">
       <c r="A222" t="s">
-        <v>39</v>
+        <v>168</v>
       </c>
       <c r="B222" t="s">
         <v>189</v>
       </c>
       <c r="C222" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="D222">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E222" t="s">
         <v>194</v>
@@ -5113,7 +5116,7 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" t="s">
-        <v>144</v>
+        <v>39</v>
       </c>
       <c r="B223" t="s">
         <v>189</v>
@@ -5130,16 +5133,16 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B224" t="s">
-        <v>2</v>
+        <v>189</v>
       </c>
       <c r="C224" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D224">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E224" t="s">
         <v>194</v>
@@ -5147,13 +5150,13 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="B225" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C225" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="D225">
         <v>3</v>
@@ -5164,13 +5167,13 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="B226" t="s">
-        <v>188</v>
+        <v>0</v>
       </c>
       <c r="C226" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="D226">
         <v>3</v>
@@ -5181,30 +5184,30 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B227" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C227" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D227">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E227" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="228" spans="1:5">
       <c r="A228" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="B228" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C228" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D228">
         <v>1</v>
@@ -5215,7 +5218,7 @@
     </row>
     <row r="229" spans="1:5">
       <c r="A229" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B229" t="s">
         <v>188</v>
@@ -5232,7 +5235,7 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B230" t="s">
         <v>188</v>
@@ -5249,7 +5252,7 @@
     </row>
     <row r="231" spans="1:5">
       <c r="A231" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B231" t="s">
         <v>188</v>
@@ -5266,7 +5269,7 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B232" t="s">
         <v>188</v>
@@ -5283,7 +5286,7 @@
     </row>
     <row r="233" spans="1:5">
       <c r="A233" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B233" t="s">
         <v>188</v>
@@ -5300,7 +5303,7 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B234" t="s">
         <v>188</v>
@@ -5317,7 +5320,7 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B235" t="s">
         <v>188</v>
@@ -5334,7 +5337,7 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B236" t="s">
         <v>188</v>
@@ -5351,7 +5354,7 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B237" t="s">
         <v>188</v>
@@ -5368,7 +5371,7 @@
     </row>
     <row r="238" spans="1:5">
       <c r="A238" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B238" t="s">
         <v>188</v>
@@ -5385,7 +5388,7 @@
     </row>
     <row r="239" spans="1:5">
       <c r="A239" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B239" t="s">
         <v>188</v>
@@ -5402,7 +5405,7 @@
     </row>
     <row r="240" spans="1:5">
       <c r="A240" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B240" t="s">
         <v>188</v>
@@ -5419,7 +5422,7 @@
     </row>
     <row r="241" spans="1:5" ht="15" customHeight="1">
       <c r="A241" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B241" t="s">
         <v>188</v>
@@ -5436,7 +5439,7 @@
     </row>
     <row r="242" spans="1:5">
       <c r="A242" t="s">
-        <v>171</v>
+        <v>111</v>
       </c>
       <c r="B242" t="s">
         <v>188</v>
@@ -5453,7 +5456,7 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="B243" t="s">
         <v>188</v>
@@ -5470,7 +5473,7 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B244" t="s">
         <v>188</v>
@@ -5487,7 +5490,7 @@
     </row>
     <row r="245" spans="1:5">
       <c r="A245" t="s">
-        <v>165</v>
+        <v>113</v>
       </c>
       <c r="B245" t="s">
         <v>188</v>
@@ -5504,7 +5507,7 @@
     </row>
     <row r="246" spans="1:5" ht="13.8" customHeight="1">
       <c r="A246" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B246" t="s">
         <v>188</v>
@@ -5521,7 +5524,7 @@
     </row>
     <row r="247" spans="1:5">
       <c r="A247" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="B247" t="s">
         <v>188</v>
@@ -5538,29 +5541,35 @@
     </row>
     <row r="248" spans="1:5">
       <c r="A248" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
       <c r="B248" t="s">
-        <v>1</v>
+        <v>188</v>
       </c>
       <c r="C248" t="s">
-        <v>200</v>
+        <v>211</v>
+      </c>
+      <c r="D248">
+        <v>1</v>
+      </c>
+      <c r="E248" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="249" spans="1:5">
       <c r="A249" t="s">
-        <v>257</v>
+        <v>172</v>
       </c>
       <c r="B249" t="s">
-        <v>254</v>
+        <v>1</v>
       </c>
       <c r="C249" t="s">
-        <v>255</v>
+        <v>200</v>
       </c>
     </row>
     <row r="250" spans="1:5">
       <c r="A250" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B250" t="s">
         <v>254</v>
@@ -5571,18 +5580,18 @@
     </row>
     <row r="251" spans="1:5">
       <c r="A251" t="s">
-        <v>288</v>
+        <v>256</v>
       </c>
       <c r="B251" t="s">
-        <v>0</v>
+        <v>254</v>
       </c>
       <c r="C251" t="s">
-        <v>181</v>
+        <v>255</v>
       </c>
     </row>
     <row r="252" spans="1:5">
       <c r="A252" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="B252" t="s">
         <v>0</v>
@@ -5593,7 +5602,7 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B253" t="s">
         <v>0</v>
@@ -5604,7 +5613,7 @@
     </row>
     <row r="254" spans="1:5">
       <c r="A254" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B254" t="s">
         <v>0</v>
@@ -5615,7 +5624,7 @@
     </row>
     <row r="255" spans="1:5">
       <c r="A255" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B255" t="s">
         <v>0</v>
@@ -5626,7 +5635,7 @@
     </row>
     <row r="256" spans="1:5">
       <c r="A256" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B256" t="s">
         <v>0</v>
@@ -5637,7 +5646,7 @@
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B257" t="s">
         <v>0</v>
@@ -5648,7 +5657,7 @@
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B258" t="s">
         <v>0</v>
@@ -5659,7 +5668,7 @@
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B259" t="s">
         <v>0</v>
@@ -5670,29 +5679,29 @@
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B260" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C260" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B261" t="s">
-        <v>267</v>
+        <v>1</v>
       </c>
       <c r="C261" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B262" t="s">
         <v>267</v>
@@ -5703,7 +5712,7 @@
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B263" t="s">
         <v>267</v>
@@ -5712,10 +5721,21 @@
         <v>188</v>
       </c>
     </row>
+    <row r="264" spans="1:3">
+      <c r="A264" t="s">
+        <v>321</v>
+      </c>
+      <c r="B264" t="s">
+        <v>267</v>
+      </c>
+      <c r="C264" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:E263">
-    <sortCondition ref="E2:E263"/>
-    <sortCondition ref="D2:D263"/>
+  <sortState ref="A2:E264">
+    <sortCondition ref="E2:E264"/>
+    <sortCondition ref="D2:D264"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>